<commit_message>
updated 2nd scenario test data and flow
</commit_message>
<xml_diff>
--- a/resources/objectrepository/objectRepository.xlsx
+++ b/resources/objectrepository/objectRepository.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Audithya\Aconex\resources\objectrepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Interview\aconex\resources\objectrepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B75614-8FF1-44C4-9EE5-DE94FA2ACB50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525F66F8-FF72-4BA9-93DC-339E90DABDAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="143">
   <si>
     <t>ScreenName</t>
   </si>
@@ -448,6 +448,12 @@
   </si>
   <si>
     <t>//div[@class='form-field']/input</t>
+  </si>
+  <si>
+    <t>date_RevisionDate</t>
+  </si>
+  <si>
+    <t>//input[@id='revisiondate_0_da']</t>
   </si>
 </sst>
 </file>
@@ -773,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,13 +1465,13 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>125</v>
+        <v>77</v>
       </c>
       <c r="B62" t="s">
-        <v>126</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>127</v>
+        <v>141</v>
+      </c>
+      <c r="C62" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1473,10 +1479,10 @@
         <v>125</v>
       </c>
       <c r="B63" t="s">
-        <v>66</v>
+        <v>126</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1484,10 +1490,10 @@
         <v>125</v>
       </c>
       <c r="B64" t="s">
-        <v>38</v>
-      </c>
-      <c r="C64" t="s">
-        <v>129</v>
+        <v>66</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1495,10 +1501,10 @@
         <v>125</v>
       </c>
       <c r="B65" t="s">
-        <v>131</v>
+        <v>38</v>
       </c>
       <c r="C65" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1506,10 +1512,10 @@
         <v>125</v>
       </c>
       <c r="B66" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C66" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1517,10 +1523,10 @@
         <v>125</v>
       </c>
       <c r="B67" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C67" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1528,10 +1534,10 @@
         <v>125</v>
       </c>
       <c r="B68" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C68" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1539,10 +1545,10 @@
         <v>125</v>
       </c>
       <c r="B69" t="s">
-        <v>59</v>
+        <v>135</v>
       </c>
       <c r="C69" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1550,9 +1556,20 @@
         <v>125</v>
       </c>
       <c r="B70" t="s">
+        <v>59</v>
+      </c>
+      <c r="C70" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>125</v>
+      </c>
+      <c r="B71" t="s">
         <v>138</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C71" t="s">
         <v>139</v>
       </c>
     </row>

</xml_diff>